<commit_message>
committing before pull from dev
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/NCR.xlsx
+++ b/Popeyes.suite/Resources/NCR.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="84">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -64,6 +64,12 @@
     <t xml:space="preserve">ProteinDisplayName</t>
   </si>
   <si>
+    <t xml:space="preserve">SidesValidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ProteinValidation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Butterfly Shrimp &amp; Tender Combo</t>
   </si>
   <si>
@@ -88,7 +94,7 @@
     <t xml:space="preserve">Mash Gravy</t>
   </si>
   <si>
-    <t xml:space="preserve">CocaCola</t>
+    <t xml:space="preserve">DietCoke</t>
   </si>
   <si>
     <t xml:space="preserve">Tndr Clsc 2P, Butterfly 8P</t>
@@ -100,6 +106,9 @@
     <t xml:space="preserve">Mash&amp;Gravy Reg</t>
   </si>
   <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
     <t xml:space="preserve">Classic Chicken Sandwich Combo</t>
   </si>
   <si>
@@ -115,15 +124,15 @@
     <t xml:space="preserve">Red Beans Rice</t>
   </si>
   <si>
-    <t xml:space="preserve">DietCoke</t>
-  </si>
-  <si>
     <t xml:space="preserve">Classic Sandwch</t>
   </si>
   <si>
     <t xml:space="preserve">Clsc San CMB, Classic Sandwich, Beans &amp; Rice Rg</t>
   </si>
   <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Classic Chicken Sandwich Dinner</t>
   </si>
   <si>
@@ -139,13 +148,13 @@
     <t xml:space="preserve">Classic Chicken Sandwich Lg Dinner</t>
   </si>
   <si>
-    <t xml:space="preserve">Large Dinner</t>
+    <t xml:space="preserve">Large Combo</t>
   </si>
   <si>
     <t xml:space="preserve">Clsc San LCMB</t>
   </si>
   <si>
-    <t xml:space="preserve">Red Beans Rice, Cajun Fries</t>
+    <t xml:space="preserve">Red Beans Rice, Mash Gravy</t>
   </si>
   <si>
     <t xml:space="preserve">Clsc San LCMB, Classic Sandwich, Beans &amp; Rice Rg</t>
@@ -166,40 +175,25 @@
     <t xml:space="preserve">Wings</t>
   </si>
   <si>
-    <t xml:space="preserve">12Pc Wings Combo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12P Wings Combo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6Pc Garlic Parmesan Wings, 6P Honey Lemon Wings</t>
+    <t xml:space="preserve">12Pc Classic Combo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6Pc Honey BBQ Wings, 6Pc Signature Hot Wings</t>
   </si>
   <si>
     <t xml:space="preserve">Fried Pickles</t>
   </si>
   <si>
-    <t xml:space="preserve">Wng GarPrm 6P, Wng Lmnppr 6P</t>
+    <t xml:space="preserve">Wng HnyBBQ 6P, Wng SigHot 6P</t>
   </si>
   <si>
     <t xml:space="preserve">12Pc Classic Combo, 6P Garlic Parmesan Wings, 6P Honey Lemon Wings</t>
   </si>
   <si>
-    <t xml:space="preserve">12 PC Wings Dinner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12Pc Wings Dinner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12P Wings Dinner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12Pc Classic Dinner, 6P Garlic Parmesan Wings, 6P Honey Lemon Wings</t>
-  </si>
-  <si>
     <t xml:space="preserve">12 PC Wings Lg Combo</t>
   </si>
   <si>
-    <t xml:space="preserve">12Pc Wings Large Combo</t>
+    <t xml:space="preserve">12Pc Classic Large Combo</t>
   </si>
   <si>
     <t xml:space="preserve">LgCmb Wng</t>
@@ -214,10 +208,7 @@
     <t xml:space="preserve">12 PC Wings ALC</t>
   </si>
   <si>
-    <t xml:space="preserve">12Pc Wings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12P Wings ALC</t>
+    <t xml:space="preserve">12Pc Classic ALC</t>
   </si>
   <si>
     <t xml:space="preserve">12Pc Classic ALC, 6P Garlic Parmesan Wings, 6P Honey Lemon Wings </t>
@@ -262,19 +253,13 @@
     <t xml:space="preserve">4PC BIC Dinner, 4PC CLASSIC</t>
   </si>
   <si>
-    <t xml:space="preserve">4 PC BIC  Lg Combo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Large Combo</t>
+    <t xml:space="preserve">4 PC BIC Lg Combo</t>
   </si>
   <si>
     <t xml:space="preserve">LgCmb BIC</t>
   </si>
   <si>
     <t xml:space="preserve">Cole Slaw, Home Mac Chs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DrPepperLarge</t>
   </si>
   <si>
     <t xml:space="preserve">LgCmb BIC, 4PC CLASSIC</t>
@@ -498,10 +483,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O1048576"/>
+  <dimension ref="A1:Q1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -519,7 +504,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="55.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="29.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="21.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -565,52 +552,64 @@
       <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>23</v>
+      <c r="P2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -618,40 +617,46 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -659,163 +664,187 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O5" s="2"/>
+      <c r="P5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O6" s="2"/>
+      <c r="P6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="L7" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="M7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="O7" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -823,40 +852,49 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="M8" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -864,80 +902,95 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="I9" s="2"/>
       <c r="K9" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>47</v>
+      <c r="B10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I10" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="K10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N10" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="O10" s="2" t="s">
-        <v>52</v>
+        <v>71</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -945,46 +998,49 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="I11" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="K11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="M11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="O11" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -995,40 +1051,49 @@
         <v>77</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>72</v>
+        <v>79</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>78</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1036,84 +1101,44 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="K13" s="2" t="s">
         <v>82</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>76</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H14" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
+      <c r="P13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Commit before pulling app changes
</commit_message>
<xml_diff>
--- a/Popeyes.suite/Resources/NCR.xlsx
+++ b/Popeyes.suite/Resources/NCR.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="93">
   <si>
     <t xml:space="preserve">TestCaseName</t>
   </si>
@@ -70,6 +70,12 @@
     <t xml:space="preserve">ProteinValidation</t>
   </si>
   <si>
+    <t xml:space="preserve">Coupons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discounts</t>
+  </si>
+  <si>
     <t xml:space="preserve">Butterfly Shrimp &amp; Tender Combo</t>
   </si>
   <si>
@@ -272,6 +278,27 @@
   </si>
   <si>
     <t xml:space="preserve">4PC ALC, 4PC CLASSIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLU Lookup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupons Discounts, Promo Lookup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classic Sandwch, Spicy Sandwch, Classic Sandwch, Spicy Sandwich, 4 Biscuit, Cajun Rice Lg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-Sandwich Family Meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classic Sandwch, Spicy Sandwch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X% Off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25% Discount</t>
   </si>
 </sst>
 </file>
@@ -483,10 +510,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q1048576"/>
+  <dimension ref="A1:S1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="Q15" activeCellId="0" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -558,58 +585,64 @@
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="P2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -617,46 +650,46 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -664,45 +697,45 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -710,47 +743,47 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -758,43 +791,43 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -802,49 +835,49 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="L7" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="O7" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -852,49 +885,49 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="M8" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -902,42 +935,42 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I9" s="2"/>
       <c r="K9" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -945,52 +978,52 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="L10" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="O10" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="P10" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -998,49 +1031,49 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="N11" s="2" t="s">
+      <c r="O11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="O11" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="P11" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1048,52 +1081,52 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="O12" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="O12" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="P12" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1101,41 +1134,123 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R14" s="1" t="n">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S15" s="0" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>